<commit_message>
Updated code and results
</commit_message>
<xml_diff>
--- a/Homework_4/Reservior.xlsx
+++ b/Homework_4/Reservior.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Systems analysis class\Gams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F0A371E-D730-4A84-8E97-E77CB8BBC72C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B8C6F7C-FDFC-464C-91EE-DDC2811AE405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="432" windowWidth="8640" windowHeight="6000" xr2:uid="{AC2A599C-7D5A-46C8-BB43-754D8C39172E}"/>
+    <workbookView xWindow="8136" yWindow="6360" windowWidth="8640" windowHeight="6000" xr2:uid="{1DA6C4AC-554A-4E08-B99A-778F1BD6FD43}"/>
   </bookViews>
   <sheets>
     <sheet name="Table of Contents" sheetId="24" r:id="rId1"/>
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DF037B-3BE9-4C58-8225-4C2EAA0BE0AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04918112-9007-492C-9E1A-3F9BDF720DFF}">
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1290,44 +1290,44 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" location="Scalar!A1" display="AddWater_PointA" xr:uid="{7871782E-0403-4C5D-BAB6-EFA03BB9DB2C}"/>
-    <hyperlink ref="A3" location="Scalar!A1" display="capacity_Reservior" xr:uid="{DFF487D9-B1B3-4B55-AE7B-DC114CCA74FF}"/>
-    <hyperlink ref="A4" location="Scalar!A1" display="EndStorage_Constraint" xr:uid="{6CF2DF68-5CB7-484A-90C2-B08BE646F203}"/>
-    <hyperlink ref="A5" location="FlowA!A1" display="FlowA" xr:uid="{51364788-4A42-44BC-9579-31E51B6947C7}"/>
-    <hyperlink ref="A6" location="Scalar!A1" display="FlowRate_A" xr:uid="{F70CA182-2371-41A0-B5D5-6498DDCA6AB9}"/>
-    <hyperlink ref="A7" location="hb!A1" display="hb" xr:uid="{2D71BF26-E38C-45A2-B8A1-5C5A1C5F74AC}"/>
-    <hyperlink ref="A8" location="ib!A1" display="ib" xr:uid="{EDCB7750-233E-4C9B-828D-97E014DB35C6}"/>
-    <hyperlink ref="A9" location="Inflow!A1" display="Inflow" xr:uid="{C4107324-A9D6-4860-8509-3F2070E4B1E9}"/>
-    <hyperlink ref="A10" location="Initial_Reservior!A1" display="Initial_Reservior" xr:uid="{6E663BCA-2169-4B7B-93EB-F9793EB9915D}"/>
-    <hyperlink ref="A11" location="Scalar!A1" display="Initial_storage" xr:uid="{60FBAB24-BCAC-4E59-B379-4E7C07E93A83}"/>
-    <hyperlink ref="A12" location="Irrigation_variable!A1" display="Irrigation_variable" xr:uid="{21265BD5-2A7E-4272-AE8B-F19586458887}"/>
-    <hyperlink ref="A13" location="Loc!A1" display="Loc" xr:uid="{7DBA2D12-01B1-4886-803D-38599211C9EE}"/>
-    <hyperlink ref="A14" location="Massbalance_pointB!A1" display="Massbalance_pointB" xr:uid="{B9596208-73F9-431C-B33F-B8350F12CFDC}"/>
-    <hyperlink ref="A15" location="Scalar!A1" display="MaxTurbine_capacity" xr:uid="{44CF9BF7-BF3F-467B-9822-841A71BE8E4A}"/>
-    <hyperlink ref="A16" location="Scalar!A1" display="Max_benefit" xr:uid="{BBCB019C-6778-49BF-A37E-5F850DE6DC43}"/>
-    <hyperlink ref="A17" location="Scalar!A1" display="Max_Z" xr:uid="{F4EF88B5-0B04-42B1-94B7-6AFCF80FBEC0}"/>
-    <hyperlink ref="A18" location="NewInitial_Reservior!A1" display="NewInitial_Reservior" xr:uid="{F858D732-E3B5-4A23-BF8B-41E5F7960DD1}"/>
-    <hyperlink ref="A19" location="NewPointA_Constraint!A1" display="NewPointA_Constraint" xr:uid="{9DA8944A-B42F-4A6F-BB20-2A0577459B38}"/>
-    <hyperlink ref="A20" location="NewReservior_Massbalance!A1" display="NewReservior_Massbalance" xr:uid="{F72AA625-FBCF-45FB-96C9-B8E9F1ADE6F8}"/>
-    <hyperlink ref="A21" location="New_Inflow!A1" display="New_Inflow" xr:uid="{3BFF214E-71B3-4491-9A50-900731996DCD}"/>
-    <hyperlink ref="A22" location="Obj_Value!A1" display="Obj_Value" xr:uid="{D0BB98B2-EC78-4FD1-AC31-8DBF7DDAF291}"/>
-    <hyperlink ref="A23" location="PointA_Constraint!A1" display="PointA_Constraint" xr:uid="{DDB8D8D2-E672-4340-BC8A-95543033BBD0}"/>
-    <hyperlink ref="A24" location="Scalar!A1" display="ReqWater_PointA" xr:uid="{76A6EA97-BF7E-43A9-B59F-3EE284845213}"/>
-    <hyperlink ref="A25" location="Reservior_capacity!A1" display="Reservior_capacity" xr:uid="{FEE8D76F-3737-4ABA-A2C1-40095B2B1560}"/>
-    <hyperlink ref="A26" location="Reservior_Massbalance!A1" display="Reservior_Massbalance" xr:uid="{4C3220C6-7DA8-4CE8-BC09-801D719083C0}"/>
-    <hyperlink ref="A27" location="RUN!A1" display="RUN" xr:uid="{675A9BB2-ADE0-4505-8841-7E615024C06C}"/>
-    <hyperlink ref="A28" location="T!A1" display="T" xr:uid="{7ED0EFE9-66AC-4115-859B-A7132E493C3F}"/>
-    <hyperlink ref="A29" location="Turbine_capacity!A1" display="Turbine_capacity" xr:uid="{736CFD1B-74E3-40D6-AD22-CC88585E3CAD}"/>
-    <hyperlink ref="A30" location="Turbine_variable!A1" display="Turbine_variable" xr:uid="{F55BA9BB-47DC-402A-B6EA-7251D8E96796}"/>
-    <hyperlink ref="A31" location="Water_PointA!A1" display="Water_PointA" xr:uid="{B81E684E-3C05-4323-8116-A3B99782D726}"/>
-    <hyperlink ref="A32" location="X!A1" display="X" xr:uid="{C41F9797-F5B3-4DDA-BFBC-8B9F3720972B}"/>
+    <hyperlink ref="A2" location="Scalar!A1" display="AddWater_PointA" xr:uid="{1F84E0CB-DA15-407D-8513-B75E46591DD6}"/>
+    <hyperlink ref="A3" location="Scalar!A1" display="capacity_Reservior" xr:uid="{E0B516D0-57E2-432F-9F5F-0E3BD87DC6B2}"/>
+    <hyperlink ref="A4" location="Scalar!A1" display="EndStorage_Constraint" xr:uid="{286CF45C-249E-41CD-9C05-C9AF8655604E}"/>
+    <hyperlink ref="A5" location="FlowA!A1" display="FlowA" xr:uid="{7CB4CBCE-04E8-4700-8152-EFF79764DCEB}"/>
+    <hyperlink ref="A6" location="Scalar!A1" display="FlowRate_A" xr:uid="{E0BE38CF-8267-47D2-9913-51CFE01A0DA7}"/>
+    <hyperlink ref="A7" location="hb!A1" display="hb" xr:uid="{ADA78FD7-7DEE-4E11-BBDE-E50B752799B9}"/>
+    <hyperlink ref="A8" location="ib!A1" display="ib" xr:uid="{1F0A55C5-BE7D-4093-A350-9B811AAECFD1}"/>
+    <hyperlink ref="A9" location="Inflow!A1" display="Inflow" xr:uid="{3AE8B942-2A72-40F2-B36F-F28AFB4DD96E}"/>
+    <hyperlink ref="A10" location="Initial_Reservior!A1" display="Initial_Reservior" xr:uid="{2F64D073-D8DA-47E0-82E8-0866A01AA850}"/>
+    <hyperlink ref="A11" location="Scalar!A1" display="Initial_storage" xr:uid="{BC82194A-57FD-46B6-9358-361D70E5B816}"/>
+    <hyperlink ref="A12" location="Irrigation_variable!A1" display="Irrigation_variable" xr:uid="{E7505773-F582-40FB-AD30-13205F77DC50}"/>
+    <hyperlink ref="A13" location="Loc!A1" display="Loc" xr:uid="{D4B0341D-643D-457E-9D8A-9D4410651420}"/>
+    <hyperlink ref="A14" location="Massbalance_pointB!A1" display="Massbalance_pointB" xr:uid="{6C6D9D0E-AEC0-4F62-B5A4-75306E0535F0}"/>
+    <hyperlink ref="A15" location="Scalar!A1" display="MaxTurbine_capacity" xr:uid="{3BD84BB2-7D3C-46E3-AFE9-04DAEC2BEBBF}"/>
+    <hyperlink ref="A16" location="Scalar!A1" display="Max_benefit" xr:uid="{DF2A482A-FED4-46E6-A314-D61A2610A3C3}"/>
+    <hyperlink ref="A17" location="Scalar!A1" display="Max_Z" xr:uid="{C3232AAB-302E-4414-AD73-5F4AF2DD8F26}"/>
+    <hyperlink ref="A18" location="NewInitial_Reservior!A1" display="NewInitial_Reservior" xr:uid="{2E8EB73A-CEED-412B-9B53-5053F7D144ED}"/>
+    <hyperlink ref="A19" location="NewPointA_Constraint!A1" display="NewPointA_Constraint" xr:uid="{86ADE020-7EE8-4D90-903D-29DBC2007EAF}"/>
+    <hyperlink ref="A20" location="NewReservior_Massbalance!A1" display="NewReservior_Massbalance" xr:uid="{65DA73B1-75E6-4449-A44C-B86D40B1E5EB}"/>
+    <hyperlink ref="A21" location="New_Inflow!A1" display="New_Inflow" xr:uid="{0D062523-B823-4914-8863-EDEFDDDE0986}"/>
+    <hyperlink ref="A22" location="Obj_Value!A1" display="Obj_Value" xr:uid="{C2986FAE-CC04-4589-9934-4EE1450804A4}"/>
+    <hyperlink ref="A23" location="PointA_Constraint!A1" display="PointA_Constraint" xr:uid="{E5EFE2DA-C298-4A79-91E2-D569A682E8C8}"/>
+    <hyperlink ref="A24" location="Scalar!A1" display="ReqWater_PointA" xr:uid="{EA9FAEAD-994C-4A91-9083-0BBB5234C19A}"/>
+    <hyperlink ref="A25" location="Reservior_capacity!A1" display="Reservior_capacity" xr:uid="{79177525-EE3C-44C5-B86B-BC4E1B056516}"/>
+    <hyperlink ref="A26" location="Reservior_Massbalance!A1" display="Reservior_Massbalance" xr:uid="{C67E4BAA-B7EA-4ED4-9595-9D5AD16E6430}"/>
+    <hyperlink ref="A27" location="RUN!A1" display="RUN" xr:uid="{C66F69D4-B2ED-47D8-8793-76F947C1F22D}"/>
+    <hyperlink ref="A28" location="T!A1" display="T" xr:uid="{A90E8E9D-74D6-40CF-96A0-5E37C45A3083}"/>
+    <hyperlink ref="A29" location="Turbine_capacity!A1" display="Turbine_capacity" xr:uid="{61DE69BA-D064-4BAF-9B59-6FA92994B1EE}"/>
+    <hyperlink ref="A30" location="Turbine_variable!A1" display="Turbine_variable" xr:uid="{012E199B-FF22-4DDF-ADA4-1A4F3785072B}"/>
+    <hyperlink ref="A31" location="Water_PointA!A1" display="Water_PointA" xr:uid="{40FD19C7-4FF1-48EC-8956-5A2146696A56}"/>
+    <hyperlink ref="A32" location="X!A1" display="X" xr:uid="{A58BA31F-8672-49DB-95A2-A9F4C9653C29}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE856911-A64E-4A21-94ED-43CF463C74DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BD7396C-3EFB-4DF6-BF9F-E3D6FC053A78}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1473,16 +1473,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{D1E67D49-4407-464B-AAE7-221B4E5434E5}"/>
+  <autoFilter ref="A3:E9" xr:uid="{18453015-B058-40A7-9A75-8C2E21774327}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{76C08B88-1D32-4E87-B47A-500CBF56D5F8}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{012D74DB-F369-46AE-BC3F-2C586199C3BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AE0A29-D4EE-40A2-850B-F2263D933DAD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BF53EB1-00F1-45B4-9815-C78405F4823D}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1543,16 +1543,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E4" xr:uid="{F530A4D0-0E90-4C9C-8A79-CA49021D897B}"/>
+  <autoFilter ref="A3:E4" xr:uid="{08ED3E02-0B46-4EEA-834B-77A36189092A}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{CEFF32A5-B9F9-43F4-8A0E-94EBB8F28C20}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{ABCF6F02-8590-4B35-839A-670E1A878376}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9201FA2B-961E-44AD-89BB-262183B79A87}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4409914A-390D-4E69-BA54-E7F7D458B477}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1698,16 +1698,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{F178E382-AC36-4526-A857-38466F1EDFF9}"/>
+  <autoFilter ref="A3:E9" xr:uid="{8C033CC8-5F3A-443B-81D8-FA4CD27A7047}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{6EAB440B-491C-497A-A00D-D4150E95F6CB}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{7CA6E868-15C2-46B1-B8D8-056E2A75E9B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{376E079E-7C03-4ECE-8D65-F2FA43936952}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97628ED6-52F6-4A2E-9AE1-0DD5CAD55D0C}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1836,16 +1836,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E8" xr:uid="{10856EF1-8BE1-48DF-A0D0-AF831E80C236}"/>
+  <autoFilter ref="A3:E8" xr:uid="{ECB448EC-79D8-4909-87AE-A55730888866}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9F87C498-8FC1-4DE5-98FA-8E7B8684CDC5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{C3A48827-F958-4CD3-9DC4-7261DC0BCBFD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9E1F33-D3B6-4561-9362-2DC29BD684C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80680A80-311B-4F0E-ACAC-CCC0D4ACF2CD}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1928,16 +1928,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B9" xr:uid="{9C68F256-AEE2-4A23-A909-60063CE42A26}"/>
+  <autoFilter ref="A3:B9" xr:uid="{A535EF9C-A90F-4F90-90F1-FC8F420A5F8B}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{EBEA71F2-6E68-4AFD-A3B1-B6095291E385}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{AB43F62D-A79E-42AF-B3EC-A1F713952C21}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC9AFA9-A485-489A-BEB9-36B4439625D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DE29C3-1369-48DB-995C-D91552F25900}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2012,16 +2012,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B8" xr:uid="{85D27602-4BB9-4F96-BA30-E468DE2884CA}"/>
+  <autoFilter ref="A3:B8" xr:uid="{5A0CB869-91E9-4522-ABD9-343F4939CF04}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{7429D606-3032-4CD0-8197-7F6D37A6A21C}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{AF931210-D006-4F7C-9FA7-4FD9127F944D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C34121D-964D-4283-8149-359200A02BC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A8D608-2318-4C60-9D0B-292961B8C309}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2167,16 +2167,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{CE8905C2-5F9B-491A-B229-4B660D00915C}"/>
+  <autoFilter ref="A3:E9" xr:uid="{23FD6C78-7CE4-41F7-AEA5-089BA7C62EFC}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{F0237969-1560-4476-9894-B6C5F83E8507}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{7B381B6B-A6C7-4B40-A1AD-2CCA4D925A70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A971E156-BCEE-4E76-A818-554F95D3E84D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51340582-76C2-40CB-823C-6E9B3834248D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2322,16 +2322,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{DE6812D1-F9FF-4008-912C-E187C215A7CA}"/>
+  <autoFilter ref="A3:E9" xr:uid="{0A4B6C8D-F472-4499-89FA-1EA219575356}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{1608A05F-11B6-4A9E-975E-28604FF0B3A7}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{1CAA7B08-0C44-4B23-9ACC-F2F990D3F219}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA74CF04-6FED-42AF-B1FA-C05B7FF516E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6D43A2-B531-4D51-B670-5831EA59EF63}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2460,16 +2460,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E8" xr:uid="{C8C48E90-A690-44A7-BD42-8CF5251212B3}"/>
+  <autoFilter ref="A3:E8" xr:uid="{A608C518-4A3F-4E42-AF53-AF3D964FF507}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{EE0574B9-6A52-4D07-9126-DD014D260F68}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9EEBB9A7-5C70-49CB-BD59-83A88D93D0B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA43257-7CCF-4E05-9712-6F212291B916}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0665B3D3-6D7B-42BD-BB57-125504B7B005}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2526,16 +2526,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A8" xr:uid="{94E082BF-070A-460B-B2CD-A40F567C9034}"/>
+  <autoFilter ref="A3:A8" xr:uid="{A72737CF-D1EA-47D2-89CD-CB48A5A3BCDE}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5F08697B-1F2C-42DF-B268-359ABB5C75C5}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{6446D913-A153-4989-A17C-7FA703B15962}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE464BF-F71B-4EDB-A424-6060EF1604D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094E51D7-C418-43E4-AB03-6EAB443C901D}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2726,14 +2726,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{20002225-D017-4264-90C3-E7BBFCB6DEA6}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{61EC08F0-C8FD-4595-9D9D-3058C9D7BF9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61521168-97AD-4C1A-AB81-D6E3BCDC605B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7E046A3-E9D5-45B7-9961-FAA570EB1B6E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2795,16 +2795,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A9" xr:uid="{9896310F-ABF5-4197-BD95-A2E7978B6D83}"/>
+  <autoFilter ref="A3:A9" xr:uid="{868625A7-BE67-495E-ABEB-70CF250EEC4E}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9157A607-D202-4B7E-AA88-3667422D5F48}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5F650B1D-D7EB-4149-B1A3-4C1BDD1C79DA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DE9290-4AF6-459D-B2FA-C9F302ABCD2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC7CC57-94BD-48CC-937F-CF517CC6450D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2950,16 +2950,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{54C602E7-A227-4C9B-8A6C-FE962311A388}"/>
+  <autoFilter ref="A3:E9" xr:uid="{16CA49C4-4DD5-471A-89FB-486EC56257B4}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{147C9069-A9AD-4251-B81C-595BE681AA84}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{5D701B10-AAEA-4031-BFD3-51102DB63331}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFA48F7-C46F-4F27-9017-82AC7172EEC4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDCF9E2-C503-424D-85C4-BBD7ABEFE168}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3327,16 +3327,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C33" xr:uid="{C353DEA4-683C-4991-888A-9392F5F0C707}"/>
+  <autoFilter ref="A3:C33" xr:uid="{E24B6097-A63D-49EA-A57F-700E418370C3}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{CBEE6924-C5DC-4A8B-8114-DAADF1FEE179}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{98423450-B63A-45B5-BE18-03DCCAE8EA2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB645F7-4525-46B7-8C9F-EE6DCE45DE45}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC2F43A9-2DF4-4C18-B959-B608032E648E}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3411,16 +3411,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B8" xr:uid="{733447C4-AB9A-40ED-9160-1DC22E5170D0}"/>
+  <autoFilter ref="A3:B8" xr:uid="{B72A61C3-A50F-4764-A9D3-5F2ED88919C4}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9A008B81-FB47-4511-8977-A8B10D73DB27}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{BB3DEB9C-97D1-4A72-9DBB-BB0D3E11BF3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7960B2DE-6A76-4B3E-AD5B-D57736042E53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49043E6-20CE-4DF0-8191-73BC02DE9521}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4067,16 +4067,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F33" xr:uid="{CADC5BE4-5CCD-4BB0-9ABA-B328B8AD97EB}"/>
+  <autoFilter ref="A3:F33" xr:uid="{9B37AB5A-2168-4757-BB55-248A4C1498AA}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{FC3DD2A2-A202-410B-A434-B47E124B75D3}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{E81415DB-C396-451A-8BA5-81311310DE07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9E9007-9405-4C19-81E9-78D1865BFC9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F6BF83-EAEF-4401-BAF6-B31E4972102B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4222,16 +4222,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E9" xr:uid="{6B158103-F34B-4988-8809-17BF9E2FF13A}"/>
+  <autoFilter ref="A3:E9" xr:uid="{FFEAF35D-F47D-4E15-97EE-F907B4791D58}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{08504685-DFE6-4289-8C8A-1437646F3120}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{83BA6B2B-A679-4E3F-A068-1E6FFB87A6E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E648630-32AC-40B5-BE18-5E6D9E24B9B0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91918C15-317B-466C-A798-E856891E5086}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4314,16 +4314,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B9" xr:uid="{B8BA6BCD-B958-4486-884E-B67FFA66C37C}"/>
+  <autoFilter ref="A3:B9" xr:uid="{B0A5FB77-222C-4B8D-BFCB-C69070D27157}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9862458E-7021-4DE2-BD88-C75F5D95F43C}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{80A4ED8C-397E-4C61-8EF7-DF399F42A4AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3D3C15-F9CF-4D79-97D3-EEC2302521AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89144588-3A45-41B8-928C-228790D05B11}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4406,16 +4406,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B9" xr:uid="{5F33A06D-EEA4-4E3B-A1CA-B9DE92F5BB6C}"/>
+  <autoFilter ref="A3:B9" xr:uid="{D767CD13-AB29-4AB9-B6C7-C0D2967ECAD6}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{E9C3906E-1522-4A5C-BCC6-112181D05924}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{6B6959A9-AEA5-4E4E-86CA-5B134AB5C913}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15DEA87-E6CE-408E-9F27-16D4183F7006}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168ABE35-4430-41FA-BE4C-BB3AB4FA2E58}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4498,16 +4498,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B9" xr:uid="{B07D1BB4-4C23-44E5-9C2C-956AC6B9652B}"/>
+  <autoFilter ref="A3:B9" xr:uid="{54BBAB38-3338-48A2-B231-7E6576871306}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{B166B0A2-177E-4AE4-B135-1080BE07EC3D}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{B89D66AA-6B69-4946-A638-CC29FA9F4253}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB649E8B-25CF-4261-B8DF-A477E38DC64C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8735DB70-F189-409C-ADCF-7B93A042AB8D}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4568,16 +4568,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E4" xr:uid="{9055D694-5B37-495D-87AC-5D6F2C98DB70}"/>
+  <autoFilter ref="A3:E4" xr:uid="{4BF87BC9-D979-42D7-8D4E-54FE3E816692}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{20359CF3-12CC-4227-8279-4811D51AE1A8}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{04CEEFEB-0A5A-4651-932B-954FB58E8BE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A35D8DE-3E21-423F-A4EA-E5431D4C9551}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1194E55A-454F-434F-A412-9B0DFAD4440A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4714,16 +4714,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:C12" xr:uid="{5C7DD87E-7E3A-40F7-9607-AF9785A7A97F}"/>
+  <autoFilter ref="A3:C12" xr:uid="{29B65827-19E7-42CA-ABC0-A6CC35E60DCB}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{DE4A09B1-3790-4FF2-A435-52328A48973C}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{F4F3173D-4024-4B97-8904-921EECEA72B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FB7B4D-1483-45BC-9E6A-8ECC328CB0BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C208159-9A86-45F0-929C-7E91B646D0A8}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4795,9 +4795,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:A8" xr:uid="{BFAA01FE-5FDF-4F03-8313-4E1287EAA050}"/>
+  <autoFilter ref="A3:A8" xr:uid="{15A62367-11B1-46D4-8A59-64BA3E7BC216}"/>
   <hyperlinks>
-    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{9DEC3D2B-7C5D-46CA-BD9C-51FC6DF54F21}"/>
+    <hyperlink ref="A1" location="'Table of Contents'!A1" display="TOC" xr:uid="{4774E67A-8941-40A9-A2CB-70D07771A506}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>